<commit_message>
ability to download via download button
</commit_message>
<xml_diff>
--- a/IAC Invoice Form (Responses).xlsx
+++ b/IAC Invoice Form (Responses).xlsx
@@ -10,14 +10,14 @@
     <sheet name="Instructor Invoices" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Instructor Invoices'!$A$1:$X$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Instructor Invoices'!$A$1:$X$15</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,21 @@
     <t>Aug 27 24 08:45:16 PM</t>
   </si>
   <si>
+    <t>Aug 28 24 10:29:22 AM</t>
+  </si>
+  <si>
+    <t>Aug 28 24 03:11:22 PM</t>
+  </si>
+  <si>
+    <t>Aug 28 24 04:06:15 PM</t>
+  </si>
+  <si>
+    <t>Aug 28 24 05:41:04 PM</t>
+  </si>
+  <si>
+    <t>Aug 28 24 06:01:16 PM</t>
+  </si>
+  <si>
     <t>jessalynnguyen001@gmail.com</t>
   </si>
   <si>
@@ -139,6 +154,21 @@
     <t>tinamchuynh@gmail.com</t>
   </si>
   <si>
+    <t>njohnp@gmail.com</t>
+  </si>
+  <si>
+    <t>jhmjr123investments@gmail.com</t>
+  </si>
+  <si>
+    <t>jenny.dd0909@gmail.com</t>
+  </si>
+  <si>
+    <t>michaelkhoale@gmail.com</t>
+  </si>
+  <si>
+    <t>jwoleary2@gmail.com</t>
+  </si>
+  <si>
     <t>Jessalyn Nguyen</t>
   </si>
   <si>
@@ -163,6 +193,21 @@
     <t>Tina Huynh</t>
   </si>
   <si>
+    <t>Dominick Pallatto</t>
+  </si>
+  <si>
+    <t>James Manley</t>
+  </si>
+  <si>
+    <t>Jenny Dong</t>
+  </si>
+  <si>
+    <t>Michael Le</t>
+  </si>
+  <si>
+    <t>James O'Leary</t>
+  </si>
+  <si>
     <t>$50.00</t>
   </si>
   <si>
@@ -181,28 +226,31 @@
     <t>$90.00</t>
   </si>
   <si>
-    <t>$20.00</t>
-  </si>
-  <si>
-    <t>$120.00</t>
+    <t>$75.00</t>
+  </si>
+  <si>
+    <t>$85.00</t>
+  </si>
+  <si>
+    <t>$150.00</t>
+  </si>
+  <si>
+    <t>$100.00</t>
+  </si>
+  <si>
+    <t>$110.00</t>
+  </si>
+  <si>
+    <t>$445.00</t>
+  </si>
+  <si>
+    <t>$43.00</t>
   </si>
   <si>
     <t>$40.00</t>
   </si>
   <si>
-    <t>$150.00</t>
-  </si>
-  <si>
-    <t>$210.00</t>
-  </si>
-  <si>
-    <t>$165.00</t>
-  </si>
-  <si>
-    <t>$505.00</t>
-  </si>
-  <si>
-    <t>$100.00</t>
+    <t>$135.00</t>
   </si>
   <si>
     <t>$115.00</t>
@@ -214,10 +262,13 @@
     <t>$565.00</t>
   </si>
   <si>
+    <t>$230.00</t>
+  </si>
+  <si>
     <t>$10.00</t>
   </si>
   <si>
-    <t>$135.00</t>
+    <t>$3.00</t>
   </si>
   <si>
     <t>$5.00</t>
@@ -589,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -698,37 +749,37 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>0</v>
@@ -755,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -772,22 +823,22 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <v>3</v>
@@ -796,13 +847,13 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -846,22 +897,22 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -870,13 +921,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -903,7 +954,7 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -920,22 +971,22 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -944,13 +995,13 @@
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -994,22 +1045,22 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1018,13 +1069,13 @@
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -1068,34 +1119,34 @@
         <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1142,22 +1193,22 @@
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H8">
         <v>2</v>
@@ -1166,13 +1217,13 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1216,22 +1267,22 @@
         <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -1240,53 +1291,423 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="K9" t="s">
-        <v>52</v>
-      </c>
-      <c r="L9">
+      <c r="E10" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9">
-        <v>0</v>
-      </c>
-      <c r="X9">
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X10"/>
+  <autoFilter ref="A1:X15"/>
   <conditionalFormatting sqref="H1:H100">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>4</formula>

</xml_diff>